<commit_message>
finished setting up feature extraction first pass
</commit_message>
<xml_diff>
--- a/url_features.xlsx
+++ b/url_features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Armand Syahtama\Dropbox\Final Year\Innovation Project\project\SEG3904-Project---Phishing-Domain-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD8EAB7-6DC9-4C5B-87C3-FD95B3051901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725BDDAD-CFFD-430C-B820-5E87197314BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2415" windowWidth="29040" windowHeight="15840" xr2:uid="{B37801CF-FA1F-254B-8147-AE37287B0B39}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B37801CF-FA1F-254B-8147-AE37287B0B39}"/>
   </bookViews>
   <sheets>
     <sheet name="url_features" sheetId="1" r:id="rId1"/>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD021159-29CB-DD4A-837D-B9DDB89DD3B3}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>